<commit_message>
Add procedural decoupler part. Remove decoupler module from LC-FL parts Add LC2 and LC3 decoupler parts (temporary, will be replaced with procedural parts in near future) Update SC-B-CM with new mass value to compensate for the now included ablator update SC-B-SM attach node names, remove extra bottom node (WARNING - SAVE BREAKING) Update SC-B-ICPS with fuel, mass, and ISP more inline with liquid-hydrogen stats Replace procedural engine fairings on SC-B parts with new generation/maintenance code - adds new options and tweakables in editor Remove example craft from distribution - they were/are/will be broken constantly during development; will recreate and replace before public release Remove some debug output from finished modules; WIP - still lots of debug stuff to be removed
</commit_message>
<xml_diff>
--- a/GameData/SSTU/Parts/ShipCore/series_b/SC-B-mass_calc.xlsx
+++ b/GameData/SSTU/Parts/ShipCore/series_b/SC-B-mass_calc.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="dv-calc" sheetId="4" r:id="rId1"/>
     <sheet name="PartInfo" sheetId="2" r:id="rId2"/>
     <sheet name="FUEL_CALC" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>Part</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>rounded</t>
+  </si>
+  <si>
+    <t>Tot DV</t>
   </si>
 </sst>
 </file>
@@ -280,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -296,6 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,7 +360,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -391,7 +395,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,6 +1468,36 @@
       <c r="R20" s="13"/>
       <c r="S20" s="14"/>
     </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21">
+        <f>B20</f>
+        <v>1330.2264899805455</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21">
+        <f>G20+B21</f>
+        <v>3002.5267818618586</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21">
+        <f>L20+G21</f>
+        <v>5326.0076560331781</v>
+      </c>
+      <c r="P21" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q21">
+        <f>Q20+L21</f>
+        <v>9460.2684950833391</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1473,7 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -2430,26 +2464,26 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>28.5</v>
+        <v>9.5</v>
       </c>
       <c r="B2">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C2">
         <f>A2/B2</f>
-        <v>5700</v>
+        <v>1900</v>
       </c>
       <c r="D2">
         <f>ROUNDUP(C2/20,0)</f>
-        <v>285</v>
+        <v>95</v>
       </c>
       <c r="E2">
         <f>9*D2</f>
-        <v>2565</v>
+        <v>855</v>
       </c>
       <c r="F2">
         <f>D2*11</f>
-        <v>3135</v>
+        <v>1045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>